<commit_message>
feat: Refactor email sending system and enhance logging functionality
</commit_message>
<xml_diff>
--- a/empresas.xlsx
+++ b/empresas.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Sending_CV\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D0816-AA30-42F6-8D56-998EFB3055CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Empresa</t>
   </si>
@@ -68,13 +74,22 @@
   </si>
   <si>
     <t>recrutamento@devcompany.com.br</t>
+  </si>
+  <si>
+    <t>Cara Core Informática</t>
+  </si>
+  <si>
+    <t>Programador Python</t>
+  </si>
+  <si>
+    <t>suporte@caracore.com.br</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +101,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,27 +152,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -181,7 +221,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -215,6 +255,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -249,9 +290,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -424,14 +466,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -453,7 +502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -464,7 +513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -475,7 +524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -486,7 +535,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -497,7 +546,21 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{0A368496-7ED6-4B58-8862-0DA0C4D77527}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>